<commit_message>
data hook updates and revising internal workflows
</commit_message>
<xml_diff>
--- a/data/primary_studies/McClellan_et_al_2021/intermediate/McClellan_2021_material_and_methods.xlsx
+++ b/data/primary_studies/McClellan_et_al_2021/intermediate/McClellan_2021_material_and_methods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/CCRCN-Data-Library/data/primary_studies/McClellan_et_al_2021/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD84886-8BE4-E349-8C3C-FE9A2BC775A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A7B2BE-AF74-AE4D-A20D-40528A279B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1440" windowWidth="25600" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,10 +286,10 @@
     <t>roots and rhizomes separated</t>
   </si>
   <si>
-    <t>not specified</t>
-  </si>
-  <si>
     <t>air dried to constant mass</t>
+  </si>
+  <si>
+    <t>none specified</t>
   </si>
 </sst>
 </file>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1421,7 +1421,7 @@
         <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>87</v>
@@ -1433,7 +1433,7 @@
         <v>60</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M4" s="2">
         <v>550</v>

</xml_diff>